<commit_message>
Update for 2024 November data release
</commit_message>
<xml_diff>
--- a/2-Config-Files/cds_config/UI-database mappings_v3.xlsx
+++ b/2-Config-Files/cds_config/UI-database mappings_v3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangf6/Documents/cds-etl/2-Config-Files/cds_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD4164D-F14E-2144-B297-5ECB238F4B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA12BC0-C686-5D43-A301-B70F529A217B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9320" yWindow="500" windowWidth="38400" windowHeight="19460" xr2:uid="{0BC66A93-5BEB-764C-8BB9-E5211772CAA1}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="151">
   <si>
     <t>Facet filters</t>
   </si>
@@ -475,13 +475,55 @@
   </si>
   <si>
     <t>Sample Type</t>
+  </si>
+  <si>
+    <t>MultiplexMicroscopy.tissue_fixative</t>
+  </si>
+  <si>
+    <t>MultiplexMicroscopy</t>
+  </si>
+  <si>
+    <t>image.organ_or_tissue</t>
+  </si>
+  <si>
+    <t>organ_or_tissue</t>
+  </si>
+  <si>
+    <t>MultiplexMicroscopy.imaging_assay_type</t>
+  </si>
+  <si>
+    <t>imaging_assay_type</t>
+  </si>
+  <si>
+    <t>proteomic.analytical_fractions</t>
+  </si>
+  <si>
+    <t>proteomic.instrument_make</t>
+  </si>
+  <si>
+    <t>proteomic.proteomic_design_description</t>
+  </si>
+  <si>
+    <t>analytical_fractions</t>
+  </si>
+  <si>
+    <t>instrument_make</t>
+  </si>
+  <si>
+    <t>proteomic_design_description</t>
+  </si>
+  <si>
+    <t>proteomic</t>
+  </si>
+  <si>
+    <t>tissue_fixative</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -524,6 +566,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF172B4D"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -551,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -567,6 +621,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,9 +641,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -625,7 +681,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -731,7 +787,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -873,7 +929,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -881,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C948E4-1DF0-6249-BEB1-83F763634681}">
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2761,6 +2817,108 @@
         <v>sample_type</v>
       </c>
     </row>
+    <row r="90" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>79</v>
+      </c>
+      <c r="B90" t="s">
+        <v>76</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E90" t="s">
+        <v>138</v>
+      </c>
+      <c r="F90" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>79</v>
+      </c>
+      <c r="B91" t="s">
+        <v>76</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="E91" t="s">
+        <v>138</v>
+      </c>
+      <c r="F91" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>79</v>
+      </c>
+      <c r="B92" t="s">
+        <v>76</v>
+      </c>
+      <c r="D92" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E92" t="s">
+        <v>149</v>
+      </c>
+      <c r="F92" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>79</v>
+      </c>
+      <c r="B93" t="s">
+        <v>76</v>
+      </c>
+      <c r="D93" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E93" t="s">
+        <v>149</v>
+      </c>
+      <c r="F93" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>79</v>
+      </c>
+      <c r="B94" t="s">
+        <v>76</v>
+      </c>
+      <c r="D94" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E94" t="s">
+        <v>149</v>
+      </c>
+      <c r="F94" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>79</v>
+      </c>
+      <c r="B95" t="s">
+        <v>76</v>
+      </c>
+      <c r="D95" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E95" t="s">
+        <v>134</v>
+      </c>
+      <c r="F95" t="s">
+        <v>140</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F39" xr:uid="{31C948E4-1DF0-6249-BEB1-83F763634681}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F83">
@@ -2774,10 +2932,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F09E50E9-33B3-FE43-9963-D716D4024E8E}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="B24" sqref="B24:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3055,6 +3213,72 @@
         <v>135</v>
       </c>
     </row>
+    <row r="24" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B25" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B27" t="s">
+        <v>149</v>
+      </c>
+      <c r="C27" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="B29" t="s">
+        <v>149</v>
+      </c>
+      <c r="C29" t="s">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C18" xr:uid="{F09E50E9-33B3-FE43-9963-D716D4024E8E}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C18">
@@ -3062,15 +3286,16 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50F4F2AB-5DF1-4CD4-A2B2-D6152C68451D}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3127,6 +3352,14 @@
         <v>73</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>45637</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>